<commit_message>
Added excel sheet for practice questions
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Suma Notes\MantraNinja\DSAlgo\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1345A101-CCEF-4A21-9DBF-09D6E81C490E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5B4C1D-FC26-4393-AC42-EFA05087F567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3936" yWindow="3276" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-170" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
+    <sheet name="validPythonCode" sheetId="3" r:id="rId3"/>
+    <sheet name="submitPythonCode" sheetId="4" r:id="rId4"/>
+    <sheet name="invalidPythonCode" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t>username</t>
   </si>
@@ -149,16 +152,45 @@
   <si>
     <t>NameError: name 'hello' is not defined on line 1</t>
   </si>
+  <si>
+    <t>questionTitle</t>
+  </si>
+  <si>
+    <t>Search the array</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>Find Numbers with Even Number of Digits</t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -171,6 +203,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -199,13 +237,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,15 +470,15 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.109375" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -457,7 +500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -479,7 +522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -503,16 +546,16 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -520,7 +563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -528,23 +571,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -552,7 +595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -560,7 +603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -568,7 +611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -576,7 +619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -584,7 +627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -592,7 +635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -603,4 +646,237 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA999A81-B0C1-4E69-8277-B2FB3354048F}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AE293B-0379-4C23-BB59-06FA968BFA5A}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE603DDD-C237-4E6E-9DD6-17BAB081D59A}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel sheets added.: Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Suma Notes\MantraNinja\DSAlgo\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5B4C1D-FC26-4393-AC42-EFA05087F567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CD05DB-1749-45AF-A4C5-74C38C9A11CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-170" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
uncommented the code for cross browser/parallel testing
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Suma Notes\MantraNinja\DSAlgo\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\git\Ds-Algo\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CD05DB-1749-45AF-A4C5-74C38C9A11CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1534A377-6171-4543-94B3-FF21F099479F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>username</t>
   </si>
@@ -237,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -249,6 +249,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,15 +471,15 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -500,7 +501,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +512,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -522,7 +523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -544,18 +545,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -563,7 +564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -571,7 +572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -579,69 +580,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -659,13 +601,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -676,7 +618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -687,7 +629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -698,7 +640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -709,7 +651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -736,13 +678,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.85546875" customWidth="1"/>
+    <col min="2" max="2" width="118.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -753,7 +695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -764,7 +706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -775,7 +717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -786,7 +728,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
@@ -809,18 +751,18 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -831,7 +773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -842,7 +784,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -853,7 +795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -864,7 +806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
added logger to home,array,linkedlist
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Suma Notes\MantraNinja\DSAlgo\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CD05DB-1749-45AF-A4C5-74C38C9A11CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72C823B-81E3-47FE-865B-936C10C3DF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>username</t>
   </si>
@@ -544,10 +544,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -577,70 +577,6 @@
       </c>
       <c r="B3" s="6" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -809,8 +745,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented Data driven testing for Login module
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\git\Ds-Algo\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Suma Notes\MantraNinja\DSAlgo\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1534A377-6171-4543-94B3-FF21F099479F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F64930-672B-4F6B-B31A-4E6EC97AC32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="loginSheet" sheetId="1" r:id="rId1"/>
     <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
     <sheet name="validPythonCode" sheetId="3" r:id="rId3"/>
     <sheet name="submitPythonCode" sheetId="4" r:id="rId4"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>username</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Numpysdet86</t>
-  </si>
-  <si>
-    <t>sdet86batch</t>
   </si>
   <si>
     <t>pythonCode</t>
@@ -167,12 +164,21 @@
   <si>
     <t>Squares of a Sorted Array</t>
   </si>
+  <si>
+    <t>sdet86batch1</t>
+  </si>
+  <si>
+    <t>Tester123$</t>
+  </si>
+  <si>
+    <t>numpy@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +216,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -234,8 +247,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -249,9 +263,10 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,19 +482,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.109375" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -498,10 +513,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,32 +524,35 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{57D8A557-E7A5-4C4D-86F5-F523C4AA7ABF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -545,45 +563,40 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -601,65 +614,65 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -678,65 +691,65 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.88671875" customWidth="1"/>
+    <col min="2" max="2" width="118.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -755,66 +768,66 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added excel reading for registration
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelFile.xlsx
+++ b/src/test/resources/ExcelData/ExcelFile.xlsx
@@ -5,26 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Suma Notes\MantraNinja\DSAlgo\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\git\Ds-Algo\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F64930-672B-4F6B-B31A-4E6EC97AC32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5823BC5-4E87-4D52-9BA3-E6D56C315409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
-    <sheet name="validPythonCode" sheetId="3" r:id="rId3"/>
-    <sheet name="submitPythonCode" sheetId="4" r:id="rId4"/>
-    <sheet name="invalidPythonCode" sheetId="6" r:id="rId5"/>
+    <sheet name="registrationSheet" sheetId="7" r:id="rId2"/>
+    <sheet name="pythonCode" sheetId="2" r:id="rId3"/>
+    <sheet name="validPythonCode" sheetId="3" r:id="rId4"/>
+    <sheet name="submitPythonCode" sheetId="4" r:id="rId5"/>
+    <sheet name="invalidPythonCode" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>username</t>
   </si>
@@ -173,12 +174,71 @@
   <si>
     <t>numpy@gmail.com</t>
   </si>
+  <si>
+    <t>NumpyTest1</t>
+  </si>
+  <si>
+    <t>Testpassword2</t>
+  </si>
+  <si>
+    <r>
+      <t>abcd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <t>Please enter a valid username</t>
+  </si>
+  <si>
+    <t>Numpyninja</t>
+  </si>
+  <si>
+    <t>lessnum</t>
+  </si>
+  <si>
+    <t>Password should contain at least 8 characters</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>password_empty</t>
+  </si>
+  <si>
+    <t>password_invalid</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>username_empty</t>
+  </si>
+  <si>
+    <t>confirmpassword_empty</t>
+  </si>
+  <si>
+    <t>username_invalid</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +283,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -251,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -264,6 +331,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -482,19 +556,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -516,7 +590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +601,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -538,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -559,6 +633,118 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA705972-4910-4164-B0B1-F30A734AC19D}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="41.21875" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -569,12 +755,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -582,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -590,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -603,7 +789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA999A81-B0C1-4E69-8277-B2FB3354048F}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -614,13 +800,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.28515625" customWidth="1"/>
+    <col min="2" max="2" width="103.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -631,7 +817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -642,7 +828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -653,7 +839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -664,7 +850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -680,7 +866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AE293B-0379-4C23-BB59-06FA968BFA5A}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -691,13 +877,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.85546875" customWidth="1"/>
+    <col min="2" max="2" width="118.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -708,7 +894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -719,7 +905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -730,7 +916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -741,7 +927,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -757,7 +943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE603DDD-C237-4E6E-9DD6-17BAB081D59A}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -765,17 +951,17 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -786,7 +972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -797,7 +983,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -808,7 +994,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -819,7 +1005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>

</xml_diff>